<commit_message>
12.b - Updating de Alta Empleado
</commit_message>
<xml_diff>
--- a/Otros/Markdown.xlsx
+++ b/Otros/Markdown.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DANY\UTN\PPP\SP\Otros\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E0B5CB0-D8D6-4982-9EF8-7805F3C59421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A811497C-ACB4-4E76-8556-013E598712FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13965" yWindow="2460" windowWidth="14655" windowHeight="11385" xr2:uid="{E294F3AA-CCD3-43CA-9AEC-691CE9BF547A}"/>
+    <workbookView xWindow="13965" yWindow="2460" windowWidth="14655" windowHeight="11385" activeTab="1" xr2:uid="{E294F3AA-CCD3-43CA-9AEC-691CE9BF547A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
   <si>
     <t>duenio@duenio.com</t>
   </si>
@@ -64,9 +64,6 @@
     <t>cuil</t>
   </si>
   <si>
-    <t>foto</t>
-  </si>
-  <si>
     <t>uid</t>
   </si>
   <si>
@@ -191,6 +188,24 @@
   </si>
   <si>
     <t>template_5p2rx0v</t>
+  </si>
+  <si>
+    <t>correo</t>
+  </si>
+  <si>
+    <t>estado</t>
+  </si>
+  <si>
+    <t>fe.creacion</t>
+  </si>
+  <si>
+    <t>img</t>
+  </si>
+  <si>
+    <t>peril</t>
+  </si>
+  <si>
+    <t>rol</t>
   </si>
 </sst>
 </file>
@@ -229,12 +244,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -250,7 +277,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -258,6 +285,8 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -575,8 +604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{975F3143-E03D-4E22-A783-266CE7D88315}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -594,16 +623,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -612,7 +641,7 @@
         <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D4" s="1"/>
     </row>
@@ -621,34 +650,34 @@
         <v>7</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -661,16 +690,16 @@
         <v>7</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D11" s="1"/>
     </row>
@@ -702,10 +731,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54FE2F9E-DB6F-48FD-A80E-F79F695920D7}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -720,47 +749,59 @@
     <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D2">
         <v>30111111</v>
       </c>
       <c r="E2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G2" t="s">
         <v>0</v>
@@ -769,21 +810,21 @@
         <v>111111</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D3">
         <v>30222222</v>
       </c>
       <c r="E3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>1</v>
@@ -792,21 +833,21 @@
         <v>222222</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D4">
         <v>30333333</v>
       </c>
       <c r="E4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>2</v>
@@ -815,21 +856,21 @@
         <v>333333</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D5">
         <v>30444444</v>
       </c>
       <c r="E5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G5" t="s">
         <v>3</v>
@@ -838,21 +879,21 @@
         <v>444444</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D6">
         <v>30555555</v>
       </c>
       <c r="E6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G6" t="s">
         <v>4</v>
@@ -861,21 +902,21 @@
         <v>555555</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D7">
         <v>30666666</v>
       </c>
       <c r="E7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G7" t="s">
         <v>5</v>
@@ -884,21 +925,21 @@
         <v>666666</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D8">
         <v>30777777</v>
       </c>
       <c r="E8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G8" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
agrego las PN a las consultas
</commit_message>
<xml_diff>
--- a/Otros/Markdown.xlsx
+++ b/Otros/Markdown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DANY\UTN\PPP\SP\Otros\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80E8ED66-6C4D-423F-8189-26B16B2EC8D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14E5E082-5F76-4F70-881C-6BFDF910E62E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{E294F3AA-CCD3-43CA-9AEC-691CE9BF547A}"/>
   </bookViews>
@@ -638,19 +638,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1198,7 +1198,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7305BBEB-8BC9-4548-8C32-A0213B1DF03B}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -1294,7 +1294,7 @@
       <c r="A3" s="16">
         <v>2</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="18" t="s">
         <v>56</v>
       </c>
       <c r="C3" s="10" t="s">
@@ -1331,8 +1331,8 @@
       <c r="Z3" s="5"/>
     </row>
     <row r="4" spans="1:26" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="17"/>
-      <c r="B4" s="20"/>
+      <c r="A4" s="20"/>
+      <c r="B4" s="21"/>
       <c r="C4" s="10" t="s">
         <v>60</v>
       </c>
@@ -1369,8 +1369,8 @@
       <c r="Z4" s="5"/>
     </row>
     <row r="5" spans="1:26" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="18"/>
-      <c r="B5" s="21"/>
+      <c r="A5" s="17"/>
+      <c r="B5" s="19"/>
       <c r="C5" s="4" t="s">
         <v>65</v>
       </c>
@@ -1406,7 +1406,7 @@
       <c r="A6" s="16">
         <v>3</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="18" t="s">
         <v>67</v>
       </c>
       <c r="C6" s="10" t="s">
@@ -1441,8 +1441,8 @@
       <c r="Z6" s="5"/>
     </row>
     <row r="7" spans="1:26" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="17"/>
-      <c r="B7" s="20"/>
+      <c r="A7" s="20"/>
+      <c r="B7" s="21"/>
       <c r="C7" s="10" t="s">
         <v>60</v>
       </c>
@@ -1475,8 +1475,8 @@
       <c r="Z7" s="5"/>
     </row>
     <row r="8" spans="1:26" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="17"/>
-      <c r="B8" s="20"/>
+      <c r="A8" s="20"/>
+      <c r="B8" s="21"/>
       <c r="C8" s="10" t="s">
         <v>65</v>
       </c>
@@ -1509,8 +1509,8 @@
       <c r="Z8" s="5"/>
     </row>
     <row r="9" spans="1:26" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="18"/>
-      <c r="B9" s="21"/>
+      <c r="A9" s="17"/>
+      <c r="B9" s="19"/>
       <c r="C9" s="4" t="s">
         <v>71</v>
       </c>
@@ -1546,7 +1546,7 @@
       <c r="A10" s="16">
         <v>4</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="18" t="s">
         <v>74</v>
       </c>
       <c r="C10" s="10" t="s">
@@ -1581,8 +1581,8 @@
       <c r="Z10" s="5"/>
     </row>
     <row r="11" spans="1:26" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="18"/>
-      <c r="B11" s="21"/>
+      <c r="A11" s="17"/>
+      <c r="B11" s="19"/>
       <c r="C11" s="4" t="s">
         <v>60</v>
       </c>
@@ -1618,7 +1618,7 @@
       <c r="A12" s="16">
         <v>5</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="18" t="s">
         <v>77</v>
       </c>
       <c r="C12" s="10" t="s">
@@ -1655,8 +1655,8 @@
       <c r="Z12" s="5"/>
     </row>
     <row r="13" spans="1:26" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="18"/>
-      <c r="B13" s="21"/>
+      <c r="A13" s="17"/>
+      <c r="B13" s="19"/>
       <c r="C13" s="4" t="s">
         <v>60</v>
       </c>
@@ -1692,7 +1692,7 @@
       <c r="A14" s="16">
         <v>6</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="18" t="s">
         <v>81</v>
       </c>
       <c r="C14" s="10" t="s">
@@ -1729,8 +1729,8 @@
       <c r="Z14" s="5"/>
     </row>
     <row r="15" spans="1:26" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="17"/>
-      <c r="B15" s="20"/>
+      <c r="A15" s="20"/>
+      <c r="B15" s="21"/>
       <c r="C15" s="10" t="s">
         <v>60</v>
       </c>
@@ -1765,8 +1765,8 @@
       <c r="Z15" s="5"/>
     </row>
     <row r="16" spans="1:26" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="18"/>
-      <c r="B16" s="21"/>
+      <c r="A16" s="17"/>
+      <c r="B16" s="19"/>
       <c r="C16" s="4" t="s">
         <v>65</v>
       </c>
@@ -1804,7 +1804,7 @@
       <c r="A17" s="16">
         <v>7</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="18" t="s">
         <v>88</v>
       </c>
       <c r="C17" s="10" t="s">
@@ -1841,8 +1841,8 @@
       <c r="Z17" s="5"/>
     </row>
     <row r="18" spans="1:26" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="18"/>
-      <c r="B18" s="21"/>
+      <c r="A18" s="17"/>
+      <c r="B18" s="19"/>
       <c r="C18" s="4" t="s">
         <v>60</v>
       </c>
@@ -1880,7 +1880,7 @@
       <c r="A19" s="16">
         <v>8</v>
       </c>
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="18" t="s">
         <v>92</v>
       </c>
       <c r="C19" s="10" t="s">
@@ -1915,8 +1915,8 @@
       <c r="Z19" s="5"/>
     </row>
     <row r="20" spans="1:26" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="18"/>
-      <c r="B20" s="21"/>
+      <c r="A20" s="17"/>
+      <c r="B20" s="19"/>
       <c r="C20" s="4" t="s">
         <v>60</v>
       </c>
@@ -1954,7 +1954,7 @@
       <c r="A21" s="16">
         <v>9</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="18" t="s">
         <v>95</v>
       </c>
       <c r="C21" s="10" t="s">
@@ -1989,8 +1989,8 @@
       <c r="Z21" s="5"/>
     </row>
     <row r="22" spans="1:26" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="18"/>
-      <c r="B22" s="21"/>
+      <c r="A22" s="17"/>
+      <c r="B22" s="19"/>
       <c r="C22" s="4" t="s">
         <v>60</v>
       </c>
@@ -2026,7 +2026,7 @@
       <c r="A23" s="16">
         <v>10</v>
       </c>
-      <c r="B23" s="19" t="s">
+      <c r="B23" s="18" t="s">
         <v>98</v>
       </c>
       <c r="C23" s="10" t="s">
@@ -2063,8 +2063,8 @@
       <c r="Z23" s="5"/>
     </row>
     <row r="24" spans="1:26" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="17"/>
-      <c r="B24" s="20"/>
+      <c r="A24" s="20"/>
+      <c r="B24" s="21"/>
       <c r="C24" s="10" t="s">
         <v>60</v>
       </c>
@@ -2097,8 +2097,8 @@
       <c r="Z24" s="5"/>
     </row>
     <row r="25" spans="1:26" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="18"/>
-      <c r="B25" s="21"/>
+      <c r="A25" s="17"/>
+      <c r="B25" s="19"/>
       <c r="C25" s="4" t="s">
         <v>65</v>
       </c>
@@ -2134,7 +2134,7 @@
       <c r="A26" s="16">
         <v>11</v>
       </c>
-      <c r="B26" s="19" t="s">
+      <c r="B26" s="18" t="s">
         <v>102</v>
       </c>
       <c r="C26" s="10" t="s">
@@ -2171,8 +2171,8 @@
       <c r="Z26" s="5"/>
     </row>
     <row r="27" spans="1:26" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="18"/>
-      <c r="B27" s="21"/>
+      <c r="A27" s="17"/>
+      <c r="B27" s="19"/>
       <c r="C27" s="4" t="s">
         <v>60</v>
       </c>
@@ -2210,7 +2210,7 @@
       <c r="A28" s="16">
         <v>12</v>
       </c>
-      <c r="B28" s="19" t="s">
+      <c r="B28" s="18" t="s">
         <v>106</v>
       </c>
       <c r="C28" s="10" t="s">
@@ -2247,8 +2247,8 @@
       <c r="Z28" s="5"/>
     </row>
     <row r="29" spans="1:26" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="18"/>
-      <c r="B29" s="21"/>
+      <c r="A29" s="17"/>
+      <c r="B29" s="19"/>
       <c r="C29" s="4" t="s">
         <v>60</v>
       </c>
@@ -2286,7 +2286,7 @@
       <c r="A30" s="16">
         <v>13</v>
       </c>
-      <c r="B30" s="19" t="s">
+      <c r="B30" s="18" t="s">
         <v>110</v>
       </c>
       <c r="C30" s="10" t="s">
@@ -2323,8 +2323,8 @@
       <c r="Z30" s="5"/>
     </row>
     <row r="31" spans="1:26" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="18"/>
-      <c r="B31" s="21"/>
+      <c r="A31" s="17"/>
+      <c r="B31" s="19"/>
       <c r="C31" s="4" t="s">
         <v>60</v>
       </c>
@@ -29492,30 +29492,30 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="B23:B25"/>
     <mergeCell ref="A26:A27"/>
     <mergeCell ref="B26:B27"/>
     <mergeCell ref="A28:A29"/>
     <mergeCell ref="B28:B29"/>
     <mergeCell ref="A30:A31"/>
     <mergeCell ref="B30:B31"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
agrego vinculacion de juegos al pedido
</commit_message>
<xml_diff>
--- a/Otros/Markdown.xlsx
+++ b/Otros/Markdown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DANY\UTN\PPP\SP\Otros\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14E5E082-5F76-4F70-881C-6BFDF910E62E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE4D5075-1F03-41B6-A212-DF333A3DA2A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{E294F3AA-CCD3-43CA-9AEC-691CE9BF547A}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="111">
   <si>
     <t>duenio@duenio.com</t>
   </si>
@@ -277,13 +277,7 @@
     <t>Al tener la mesa asignada, se muestra el botón de “consulta al mozo”, que permite hacer una consulta rápida al mozo (con número de mesa y la consulta).</t>
   </si>
   <si>
-    <t>ESTA HECHO</t>
-  </si>
-  <si>
     <t>Verificar que le llegue a todos los mozos la consulta realizada. (push notification*A)</t>
-  </si>
-  <si>
-    <t>FALTA</t>
   </si>
   <si>
     <t>El mozo responde la consulta. Se verifica en el cliente.</t>
@@ -638,19 +632,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1198,8 +1192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7305BBEB-8BC9-4548-8C32-A0213B1DF03B}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1294,7 +1288,7 @@
       <c r="A3" s="16">
         <v>2</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="19" t="s">
         <v>56</v>
       </c>
       <c r="C3" s="10" t="s">
@@ -1331,8 +1325,8 @@
       <c r="Z3" s="5"/>
     </row>
     <row r="4" spans="1:26" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="20"/>
-      <c r="B4" s="21"/>
+      <c r="A4" s="17"/>
+      <c r="B4" s="20"/>
       <c r="C4" s="10" t="s">
         <v>60</v>
       </c>
@@ -1369,8 +1363,8 @@
       <c r="Z4" s="5"/>
     </row>
     <row r="5" spans="1:26" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="17"/>
-      <c r="B5" s="19"/>
+      <c r="A5" s="18"/>
+      <c r="B5" s="21"/>
       <c r="C5" s="4" t="s">
         <v>65</v>
       </c>
@@ -1406,7 +1400,7 @@
       <c r="A6" s="16">
         <v>3</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="19" t="s">
         <v>67</v>
       </c>
       <c r="C6" s="10" t="s">
@@ -1441,8 +1435,8 @@
       <c r="Z6" s="5"/>
     </row>
     <row r="7" spans="1:26" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="20"/>
-      <c r="B7" s="21"/>
+      <c r="A7" s="17"/>
+      <c r="B7" s="20"/>
       <c r="C7" s="10" t="s">
         <v>60</v>
       </c>
@@ -1475,8 +1469,8 @@
       <c r="Z7" s="5"/>
     </row>
     <row r="8" spans="1:26" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="20"/>
-      <c r="B8" s="21"/>
+      <c r="A8" s="17"/>
+      <c r="B8" s="20"/>
       <c r="C8" s="10" t="s">
         <v>65</v>
       </c>
@@ -1509,8 +1503,8 @@
       <c r="Z8" s="5"/>
     </row>
     <row r="9" spans="1:26" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="17"/>
-      <c r="B9" s="19"/>
+      <c r="A9" s="18"/>
+      <c r="B9" s="21"/>
       <c r="C9" s="4" t="s">
         <v>71</v>
       </c>
@@ -1546,7 +1540,7 @@
       <c r="A10" s="16">
         <v>4</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="19" t="s">
         <v>74</v>
       </c>
       <c r="C10" s="10" t="s">
@@ -1581,8 +1575,8 @@
       <c r="Z10" s="5"/>
     </row>
     <row r="11" spans="1:26" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="17"/>
-      <c r="B11" s="19"/>
+      <c r="A11" s="18"/>
+      <c r="B11" s="21"/>
       <c r="C11" s="4" t="s">
         <v>60</v>
       </c>
@@ -1593,7 +1587,9 @@
         <v>73</v>
       </c>
       <c r="F11" s="9"/>
-      <c r="G11" s="5"/>
+      <c r="G11" s="5" t="s">
+        <v>102</v>
+      </c>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
@@ -1618,7 +1614,7 @@
       <c r="A12" s="16">
         <v>5</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="19" t="s">
         <v>77</v>
       </c>
       <c r="C12" s="10" t="s">
@@ -1655,8 +1651,8 @@
       <c r="Z12" s="5"/>
     </row>
     <row r="13" spans="1:26" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="17"/>
-      <c r="B13" s="19"/>
+      <c r="A13" s="18"/>
+      <c r="B13" s="21"/>
       <c r="C13" s="4" t="s">
         <v>60</v>
       </c>
@@ -1667,7 +1663,9 @@
         <v>73</v>
       </c>
       <c r="F13" s="9"/>
-      <c r="G13" s="5"/>
+      <c r="G13" s="5" t="s">
+        <v>102</v>
+      </c>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
@@ -1692,7 +1690,7 @@
       <c r="A14" s="16">
         <v>6</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="19" t="s">
         <v>81</v>
       </c>
       <c r="C14" s="10" t="s">
@@ -1706,7 +1704,7 @@
       </c>
       <c r="F14" s="12"/>
       <c r="G14" s="5" t="s">
-        <v>83</v>
+        <v>106</v>
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
@@ -1729,20 +1727,20 @@
       <c r="Z14" s="5"/>
     </row>
     <row r="15" spans="1:26" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="20"/>
-      <c r="B15" s="21"/>
+      <c r="A15" s="17"/>
+      <c r="B15" s="20"/>
       <c r="C15" s="10" t="s">
         <v>60</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E15" s="15" t="s">
         <v>73</v>
       </c>
       <c r="F15" s="12"/>
       <c r="G15" s="5" t="s">
-        <v>85</v>
+        <v>106</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
@@ -1765,20 +1763,20 @@
       <c r="Z15" s="5"/>
     </row>
     <row r="16" spans="1:26" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="17"/>
-      <c r="B16" s="19"/>
+      <c r="A16" s="18"/>
+      <c r="B16" s="21"/>
       <c r="C16" s="4" t="s">
         <v>65</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E16" s="14" t="s">
         <v>73</v>
       </c>
       <c r="F16" s="9"/>
       <c r="G16" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
@@ -1804,20 +1802,20 @@
       <c r="A17" s="16">
         <v>7</v>
       </c>
-      <c r="B17" s="18" t="s">
-        <v>88</v>
+      <c r="B17" s="19" t="s">
+        <v>86</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>57</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E17" s="11" t="s">
         <v>55</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
@@ -1841,19 +1839,19 @@
       <c r="Z17" s="5"/>
     </row>
     <row r="18" spans="1:26" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="17"/>
-      <c r="B18" s="19"/>
+      <c r="A18" s="18"/>
+      <c r="B18" s="21"/>
       <c r="C18" s="4" t="s">
         <v>60</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>55</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
@@ -1880,14 +1878,14 @@
       <c r="A19" s="16">
         <v>8</v>
       </c>
-      <c r="B19" s="18" t="s">
-        <v>92</v>
+      <c r="B19" s="19" t="s">
+        <v>90</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>57</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E19" s="11" t="s">
         <v>55</v>
@@ -1915,20 +1913,20 @@
       <c r="Z19" s="5"/>
     </row>
     <row r="20" spans="1:26" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="17"/>
-      <c r="B20" s="19"/>
+      <c r="A20" s="18"/>
+      <c r="B20" s="21"/>
       <c r="C20" s="4" t="s">
         <v>60</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E20" s="14" t="s">
         <v>73</v>
       </c>
       <c r="F20" s="9"/>
       <c r="G20" s="5" t="s">
-        <v>85</v>
+        <v>102</v>
       </c>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
@@ -1954,14 +1952,14 @@
       <c r="A21" s="16">
         <v>9</v>
       </c>
-      <c r="B21" s="18" t="s">
-        <v>95</v>
+      <c r="B21" s="19" t="s">
+        <v>93</v>
       </c>
       <c r="C21" s="10" t="s">
         <v>57</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E21" s="11" t="s">
         <v>55</v>
@@ -1989,13 +1987,13 @@
       <c r="Z21" s="5"/>
     </row>
     <row r="22" spans="1:26" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="17"/>
-      <c r="B22" s="19"/>
+      <c r="A22" s="18"/>
+      <c r="B22" s="21"/>
       <c r="C22" s="4" t="s">
         <v>60</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E22" s="14" t="s">
         <v>73</v>
@@ -2026,22 +2024,24 @@
       <c r="A23" s="16">
         <v>10</v>
       </c>
-      <c r="B23" s="18" t="s">
-        <v>98</v>
+      <c r="B23" s="19" t="s">
+        <v>96</v>
       </c>
       <c r="C23" s="10" t="s">
         <v>57</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E23" s="11" t="s">
         <v>55</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
-      <c r="G23" s="5"/>
+      <c r="G23" s="5" t="s">
+        <v>102</v>
+      </c>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
@@ -2063,13 +2063,13 @@
       <c r="Z23" s="5"/>
     </row>
     <row r="24" spans="1:26" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="20"/>
-      <c r="B24" s="21"/>
+      <c r="A24" s="17"/>
+      <c r="B24" s="20"/>
       <c r="C24" s="10" t="s">
         <v>60</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E24" s="11" t="s">
         <v>55</v>
@@ -2097,13 +2097,13 @@
       <c r="Z24" s="5"/>
     </row>
     <row r="25" spans="1:26" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="17"/>
-      <c r="B25" s="19"/>
+      <c r="A25" s="18"/>
+      <c r="B25" s="21"/>
       <c r="C25" s="4" t="s">
         <v>65</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>55</v>
@@ -2134,21 +2134,21 @@
       <c r="A26" s="16">
         <v>11</v>
       </c>
-      <c r="B26" s="18" t="s">
-        <v>102</v>
+      <c r="B26" s="19" t="s">
+        <v>100</v>
       </c>
       <c r="C26" s="10" t="s">
         <v>57</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E26" s="14" t="s">
         <v>73</v>
       </c>
       <c r="F26" s="12"/>
       <c r="G26" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
@@ -2171,20 +2171,20 @@
       <c r="Z26" s="5"/>
     </row>
     <row r="27" spans="1:26" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="17"/>
-      <c r="B27" s="19"/>
+      <c r="A27" s="18"/>
+      <c r="B27" s="21"/>
       <c r="C27" s="4" t="s">
         <v>60</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E27" s="14" t="s">
         <v>73</v>
       </c>
       <c r="F27" s="9"/>
       <c r="G27" s="5" t="s">
-        <v>85</v>
+        <v>102</v>
       </c>
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
@@ -2210,21 +2210,21 @@
       <c r="A28" s="16">
         <v>12</v>
       </c>
-      <c r="B28" s="18" t="s">
-        <v>106</v>
+      <c r="B28" s="19" t="s">
+        <v>104</v>
       </c>
       <c r="C28" s="10" t="s">
         <v>57</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E28" s="14" t="s">
         <v>73</v>
       </c>
       <c r="F28" s="12"/>
       <c r="G28" s="5" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
@@ -2247,20 +2247,20 @@
       <c r="Z28" s="5"/>
     </row>
     <row r="29" spans="1:26" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="17"/>
-      <c r="B29" s="19"/>
+      <c r="A29" s="18"/>
+      <c r="B29" s="21"/>
       <c r="C29" s="4" t="s">
         <v>60</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E29" s="14" t="s">
         <v>73</v>
       </c>
       <c r="F29" s="9"/>
       <c r="G29" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
@@ -2286,21 +2286,21 @@
       <c r="A30" s="16">
         <v>13</v>
       </c>
-      <c r="B30" s="18" t="s">
-        <v>110</v>
+      <c r="B30" s="19" t="s">
+        <v>108</v>
       </c>
       <c r="C30" s="10" t="s">
         <v>57</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E30" s="14" t="s">
         <v>73</v>
       </c>
       <c r="F30" s="12"/>
       <c r="G30" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
@@ -2323,20 +2323,20 @@
       <c r="Z30" s="5"/>
     </row>
     <row r="31" spans="1:26" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="17"/>
-      <c r="B31" s="19"/>
+      <c r="A31" s="18"/>
+      <c r="B31" s="21"/>
       <c r="C31" s="4" t="s">
         <v>60</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E31" s="14" t="s">
         <v>73</v>
       </c>
       <c r="F31" s="9"/>
       <c r="G31" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
@@ -29492,30 +29492,30 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="A6:A9"/>
     <mergeCell ref="B6:B9"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B10:B11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:B31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>